<commit_message>
feat(import/export): add import/export for the competitor items
</commit_message>
<xml_diff>
--- a/src/stories/massUpload/source/personnels.xlsx
+++ b/src/stories/massUpload/source/personnels.xlsx
@@ -6,12 +6,13 @@
   </bookViews>
   <sheets>
     <sheet name="Personnel" sheetId="1" r:id="rId4"/>
+    <sheet name="Position" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="816">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="841">
   <si>
     <t>ID</t>
   </si>
@@ -3764,6 +3765,81 @@
   </si>
   <si>
     <t>LULU HYPER MARKET -FUJEIRAH| AL MADINA SUPER MARKET| SAFEER SUPERMARKET FUJ| CITY MARKET - FUJ| EMIRATES GALLERY| SAJIDA DIBBA BR.| SAJIDA FUJAIRAH BR.| SAJIDA MAIN BRANCH KHORFAKKAN| SAJIDA QIDFA BR.| SAJIDA W/H| LULU EXPRESS SUPERMARKET - AL MIRBA| PALM DISCOUNT WAHAT KALBA DISCOUNTS LLC| SAJIDA SUPERMARKET (KALBA)| PALM DISCOUNT CENTER DHAID BR.| SAJIDA FUJAIRAH BR.</t>
+  </si>
+  <si>
+    <t>Name (EN)</t>
+  </si>
+  <si>
+    <t>Name (AR)</t>
+  </si>
+  <si>
+    <t>مدير التسويق</t>
+  </si>
+  <si>
+    <t>سكرتير / محلل ومنسق المبيعات</t>
+  </si>
+  <si>
+    <t>SALES MANAGER</t>
+  </si>
+  <si>
+    <t>مدير مبيعات</t>
+  </si>
+  <si>
+    <t>مسؤول منطقة</t>
+  </si>
+  <si>
+    <t>المدير العام</t>
+  </si>
+  <si>
+    <t>مدبر مبيعات ميداني</t>
+  </si>
+  <si>
+    <t>مدير مبيعات كبار العملاء</t>
+  </si>
+  <si>
+    <t>مدير عام المبيعات</t>
+  </si>
+  <si>
+    <t>مدير سوق</t>
+  </si>
+  <si>
+    <t>مشرف المبيعات</t>
+  </si>
+  <si>
+    <t>تنفيذي مبيعات</t>
+  </si>
+  <si>
+    <t>مندوب ومروج المبيعات</t>
+  </si>
+  <si>
+    <t>عامل الرفوف</t>
+  </si>
+  <si>
+    <t>مروج</t>
+  </si>
+  <si>
+    <t>مندوب مبيعات</t>
+  </si>
+  <si>
+    <t>مسؤول تحميل بيانات</t>
+  </si>
+  <si>
+    <t>MASTER UPLOADER</t>
+  </si>
+  <si>
+    <t>مسؤول تحميل البيانات الرئيسي</t>
+  </si>
+  <si>
+    <t>مسؤول المروجين</t>
+  </si>
+  <si>
+    <t>Customer Success</t>
+  </si>
+  <si>
+    <t>مسؤول نجاح العملاء</t>
+  </si>
+  <si>
+    <t>TRADE MARKETER</t>
   </si>
 </sst>
 </file>
@@ -3847,7 +3923,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3860,8 +3936,20 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="16"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -3884,13 +3972,118 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -3993,6 +4186,39 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4014,6 +4240,10 @@
       <rgbColor rgb="ff0563c1"/>
       <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ff222222"/>
+      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -5200,7 +5430,7 @@
       <c r="H3" s="8"/>
       <c r="I3" s="7"/>
       <c r="J3" t="s" s="9">
-        <f>HYPERLINK("mailto:abdulsalam@alalali.com","abdulsalam@alalali.com")</f>
+        <f t="shared" si="0" ref="J3:L14">HYPERLINK("mailto:abdulsalam@alalali.com","abdulsalam@alalali.com")</f>
         <v>26</v>
       </c>
       <c r="K3" s="7"/>
@@ -5315,12 +5545,12 @@
       <c r="H6" s="8"/>
       <c r="I6" s="7"/>
       <c r="J6" t="s" s="9">
-        <f t="shared" si="4" ref="J6:L10">HYPERLINK("mailto:nasimakhter@alalali.com","nasimakhter@alalali.com")</f>
+        <f>HYPERLINK("mailto:nasimakhter@alalali.com","nasimakhter@alalali.com")</f>
         <v>48</v>
       </c>
       <c r="K6" s="7"/>
       <c r="L6" t="s" s="9">
-        <f>HYPERLINK("mailto:abdulsalam@alalali.com","abdulsalam@alalali.com")</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="M6" t="s" s="6">
@@ -5359,7 +5589,7 @@
       </c>
       <c r="K7" s="7"/>
       <c r="L7" t="s" s="9">
-        <f>HYPERLINK("mailto:abdulsalam@alalali.com","abdulsalam@alalali.com")</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="M7" t="s" s="6">
@@ -5398,7 +5628,7 @@
       </c>
       <c r="K8" s="12"/>
       <c r="L8" t="s" s="9">
-        <f>HYPERLINK("mailto:abdulsalam@alalali.com","abdulsalam@alalali.com")</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="M8" t="s" s="11">
@@ -5473,12 +5703,12 @@
       <c r="H10" s="8"/>
       <c r="I10" s="7"/>
       <c r="J10" t="s" s="9">
-        <f>HYPERLINK("mailto:arshadkhan@alalali.com","arshadkhan@alalali.com")</f>
+        <f t="shared" si="12" ref="J10:L70">HYPERLINK("mailto:arshadkhan@alalali.com","arshadkhan@alalali.com")</f>
         <v>71</v>
       </c>
       <c r="K10" s="7"/>
       <c r="L10" t="s" s="9">
-        <f t="shared" si="4"/>
+        <f>HYPERLINK("mailto:nasimakhter@alalali.com","nasimakhter@alalali.com")</f>
         <v>48</v>
       </c>
       <c r="M10" t="s" s="6">
@@ -5610,7 +5840,7 @@
         <v>971558300915</v>
       </c>
       <c r="L13" t="s" s="9">
-        <f>HYPERLINK("mailto:abdulsalam@alalali.com","abdulsalam@alalali.com")</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="M13" t="s" s="6">
@@ -5656,7 +5886,7 @@
         <v>971558300317</v>
       </c>
       <c r="L14" t="s" s="9">
-        <f>HYPERLINK("mailto:abdulsalam@alalali.com","abdulsalam@alalali.com")</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="M14" t="s" s="6">
@@ -8197,7 +8427,7 @@
       </c>
       <c r="K70" s="7"/>
       <c r="L70" t="s" s="9">
-        <f>HYPERLINK("mailto:arshadkhan@alalali.com","arshadkhan@alalali.com")</f>
+        <f t="shared" si="12"/>
         <v>71</v>
       </c>
       <c r="M70" t="s" s="6">
@@ -12247,4 +12477,305 @@
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="15.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="5.49219" style="34" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="34" customWidth="1"/>
+    <col min="3" max="3" width="16.3516" style="34" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="34" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="34" customWidth="1"/>
+    <col min="6" max="256" width="16.3516" style="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="16.55" customHeight="1">
+      <c r="A1" t="s" s="35">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="35">
+        <v>816</v>
+      </c>
+      <c r="C1" t="s" s="35">
+        <v>817</v>
+      </c>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+    </row>
+    <row r="2" ht="16.55" customHeight="1">
+      <c r="A2" s="37">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="38">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s" s="39">
+        <v>818</v>
+      </c>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+    </row>
+    <row r="3" ht="16.35" customHeight="1">
+      <c r="A3" s="41">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="42">
+        <v>80</v>
+      </c>
+      <c r="C3" t="s" s="43">
+        <v>819</v>
+      </c>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+    </row>
+    <row r="4" ht="16.35" customHeight="1">
+      <c r="A4" s="41">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s" s="42">
+        <v>820</v>
+      </c>
+      <c r="C4" t="s" s="43">
+        <v>821</v>
+      </c>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+    </row>
+    <row r="5" ht="16.35" customHeight="1">
+      <c r="A5" s="41">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="42">
+        <v>109</v>
+      </c>
+      <c r="C5" t="s" s="43">
+        <v>822</v>
+      </c>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+    </row>
+    <row r="6" ht="16.35" customHeight="1">
+      <c r="A6" s="41">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s" s="42">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s" s="43">
+        <v>823</v>
+      </c>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+    </row>
+    <row r="7" ht="16.35" customHeight="1">
+      <c r="A7" s="41">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s" s="42">
+        <v>72</v>
+      </c>
+      <c r="C7" t="s" s="43">
+        <v>824</v>
+      </c>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+    </row>
+    <row r="8" ht="16.35" customHeight="1">
+      <c r="A8" s="41">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s" s="42">
+        <v>102</v>
+      </c>
+      <c r="C8" t="s" s="43">
+        <v>825</v>
+      </c>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+    </row>
+    <row r="9" ht="16.35" customHeight="1">
+      <c r="A9" s="41">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s" s="42">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s" s="43">
+        <v>826</v>
+      </c>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+    </row>
+    <row r="10" ht="16.35" customHeight="1">
+      <c r="A10" s="41">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s" s="42">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s" s="43">
+        <v>827</v>
+      </c>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+    </row>
+    <row r="11" ht="16.35" customHeight="1">
+      <c r="A11" s="41">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s" s="42">
+        <v>427</v>
+      </c>
+      <c r="C11" t="s" s="43">
+        <v>828</v>
+      </c>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+    </row>
+    <row r="12" ht="16.35" customHeight="1">
+      <c r="A12" s="41">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s" s="42">
+        <v>118</v>
+      </c>
+      <c r="C12" t="s" s="43">
+        <v>829</v>
+      </c>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+    </row>
+    <row r="13" ht="16.35" customHeight="1">
+      <c r="A13" s="41">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s" s="42">
+        <v>160</v>
+      </c>
+      <c r="C13" t="s" s="43">
+        <v>830</v>
+      </c>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+    </row>
+    <row r="14" ht="16.35" customHeight="1">
+      <c r="A14" s="41">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s" s="42">
+        <v>344</v>
+      </c>
+      <c r="C14" t="s" s="43">
+        <v>831</v>
+      </c>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+    </row>
+    <row r="15" ht="16.35" customHeight="1">
+      <c r="A15" s="41">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s" s="42">
+        <v>258</v>
+      </c>
+      <c r="C15" t="s" s="43">
+        <v>832</v>
+      </c>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+    </row>
+    <row r="16" ht="16.35" customHeight="1">
+      <c r="A16" s="41">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s" s="42">
+        <v>181</v>
+      </c>
+      <c r="C16" t="s" s="43">
+        <v>833</v>
+      </c>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+    </row>
+    <row r="17" ht="16.35" customHeight="1">
+      <c r="A17" s="41">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s" s="42">
+        <v>768</v>
+      </c>
+      <c r="C17" t="s" s="43">
+        <v>834</v>
+      </c>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+    </row>
+    <row r="18" ht="16.35" customHeight="1">
+      <c r="A18" s="41">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s" s="42">
+        <v>835</v>
+      </c>
+      <c r="C18" t="s" s="43">
+        <v>836</v>
+      </c>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+    </row>
+    <row r="19" ht="16.35" customHeight="1">
+      <c r="A19" s="41">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s" s="42">
+        <v>421</v>
+      </c>
+      <c r="C19" t="s" s="43">
+        <v>837</v>
+      </c>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+    </row>
+    <row r="20" ht="16.35" customHeight="1">
+      <c r="A20" s="41">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s" s="42">
+        <v>838</v>
+      </c>
+      <c r="C20" t="s" s="43">
+        <v>839</v>
+      </c>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+    </row>
+    <row r="21" ht="16.35" customHeight="1">
+      <c r="A21" s="41">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s" s="42">
+        <v>840</v>
+      </c>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>